<commit_message>
1. Finish major part of the writer design. 2. Find a problem in data type converting during read and write data. So commit the code for back up.
Signed-off-by: Spark-Liang <369453502@qq.com>
</commit_message>
<xml_diff>
--- a/test/xl_transform/reader_test/test_data/DataFrameReader/excel/ReadWithTypeHint/Source.xlsx
+++ b/test/xl_transform/reader_test/test_data/DataFrameReader/excel/ReadWithTypeHint/Source.xlsx
@@ -5,35 +5,26 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\ProjectData\ExcelTransformer\test\reader_test\test_data\DataFrameReader\excel\ReadWithTypeHint\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\ProjectData\ExcelTransformer\test\xl_transform\reader_test\test_data\DataFrameReader\excel\ReadWithTypeHint\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="7920"/>
   </bookViews>
   <sheets>
-    <sheet name="Source" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Date_1</t>
   </si>
   <si>
     <t>Date_2</t>
-  </si>
-  <si>
-    <t>str</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>float</t>
   </si>
   <si>
     <t>decimal_2</t>
@@ -634,7 +625,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -645,9 +636,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -974,19 +962,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.125" customWidth="1"/>
+    <col min="1" max="1" width="23.75" customWidth="1"/>
     <col min="2" max="2" width="16.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -996,17 +984,8 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>43830.515972222223</v>
       </c>
@@ -1014,19 +993,10 @@
         <v>43819</v>
       </c>
       <c r="C2" s="4">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>30</v>
-      </c>
-      <c r="E2">
-        <v>40</v>
-      </c>
-      <c r="F2" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>43830.377789351849</v>
       </c>
@@ -1034,19 +1004,10 @@
         <v>43820</v>
       </c>
       <c r="C3" s="4">
-        <v>0.65607004899999999</v>
-      </c>
-      <c r="D3">
-        <v>-30</v>
-      </c>
-      <c r="E3">
-        <v>0.88585444899999999</v>
-      </c>
-      <c r="F3" s="5">
         <v>-10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>43831.377789351849</v>
       </c>
@@ -1054,15 +1015,6 @@
         <v>43821</v>
       </c>
       <c r="C4" s="4">
-        <v>-0.34459226500000001</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>-2.7395487E-2</v>
-      </c>
-      <c r="F4" s="5">
         <v>12.35</v>
       </c>
     </row>

</xml_diff>